<commit_message>
New data. Good qpcr figure
</commit_message>
<xml_diff>
--- a/data/Pride_qpcr/Cocktail 8_(SDS1+Ump).xlsx
+++ b/data/Pride_qpcr/Cocktail 8_(SDS1+Ump).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poojaghatbale/Documents/UCSD Health/Growth Curve Experiments/Final Data/qPCR data/Cocktail qPCR/SDS1+Ump/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1D3D874-571A-5846-9567-78D2465E8301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C123FA-FCBD-0E47-9046-3A14665AC6DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="2960" windowWidth="23440" windowHeight="11700" activeTab="1" xr2:uid="{411C750F-0487-0B40-8B44-99190A34A317}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="SDS1" sheetId="1" r:id="rId1"/>
     <sheet name="Ump" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +106,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,10 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D07DEED-B3B9-744E-A7D9-8C349A92B215}">
   <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,307 +853,515 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FFB782-4860-7C4F-98F8-8712A8CCB7F7}">
-  <dimension ref="B2:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>9.2643840000000033</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="3">
+        <v>9.2643839999999997</v>
+      </c>
+      <c r="D4" s="3">
         <v>8.563291999999997</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E4" s="3">
+        <v>7.7949720000000013</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>8.6977479999999971</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>8.3616080000000039</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="J4" s="3">
+        <v>8.4448426666666663</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>12.574562666666669</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>13.57658</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" s="3">
+        <v>13.781465333333333</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>8.5953053333333358</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>7.1290946666666741</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="J5" s="3">
+        <v>8.816197333333335</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>9.363625333333335</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>9.5332960000000035</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E6" s="3">
+        <v>12.917105333333332</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>9.5765139999999995</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>8.4416413333333296</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="J6" s="3">
+        <v>8.8738213333333391</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>9.6357386666666649</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>8.1983400000000017</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E7" s="3">
+        <v>11.755021333333303</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>8.9058346666666637</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>7.5772813333333247</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="J7" s="3">
+        <v>8.2271519999999967</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>8.9138380000000002</v>
+        <f>AVERAGE(C4:E4)</f>
+        <v>8.5408826666666666</v>
       </c>
       <c r="D12">
-        <v>820045594.85942543</v>
+        <f>10^C12</f>
+        <v>347442280.28645116</v>
       </c>
       <c r="E12">
-        <v>0.49574690743564342</v>
+        <f>STDEV(C4:E4)</f>
+        <v>0.73496227120943558</v>
       </c>
       <c r="F12">
-        <v>0.35054600000000313</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+        <f>E12/SQRT(COUNT(C4:E4))</f>
+        <v>0.42433066512698642</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13">
-        <v>13.075571333333334</v>
+        <f t="shared" ref="C13:C15" si="0">AVERAGE(C5:E5)</f>
+        <v>13.310869333333335</v>
       </c>
       <c r="D13">
-        <v>11900667828502.852</v>
+        <f t="shared" ref="D13:D15" si="1">10^C13</f>
+        <v>20458290132535.406</v>
       </c>
       <c r="E13">
-        <v>0.70853325126645961</v>
+        <f t="shared" ref="E13:E15" si="2">STDEV(C5:E5)</f>
+        <v>0.64583676767981357</v>
       </c>
       <c r="F13">
-        <v>0.50100866666666555</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F13:F15" si="3">E13/SQRT(COUNT(C5:E5))</f>
+        <v>0.37287403167249816</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14">
-        <v>9.4484606666666693</v>
+        <f t="shared" si="0"/>
+        <v>10.604675555555557</v>
       </c>
       <c r="D14">
-        <v>2808411008.10674</v>
+        <f t="shared" si="1"/>
+        <v>40241629250.894669</v>
       </c>
       <c r="E14">
-        <v>0.11997527896844362</v>
+        <f t="shared" si="2"/>
+        <v>2.0044190284585732</v>
       </c>
       <c r="F14">
-        <v>8.4835333333334262E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>1.1572518656493656</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15">
-        <v>8.9170393333333333</v>
+        <f t="shared" si="0"/>
+        <v>9.8630333333333233</v>
       </c>
       <c r="D15">
-        <v>826112765.85676718</v>
+        <f t="shared" si="1"/>
+        <v>7295135003.3619547</v>
       </c>
       <c r="E15">
-        <v>1.0163943444684993</v>
+        <f t="shared" si="2"/>
+        <v>1.7892016867423617</v>
       </c>
       <c r="F15">
-        <v>0.71869933333333147</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+        <f t="shared" si="3"/>
+        <v>1.032996075475235</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="C18" s="1"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20">
-        <v>8.5296780000000005</v>
+        <f>AVERAGE(H4:J4)</f>
+        <v>8.5013995555555564</v>
       </c>
       <c r="D20">
-        <v>338593019.21534097</v>
+        <f>10^C20</f>
+        <v>317248484.07197613</v>
       </c>
       <c r="E20">
-        <v>0.23768687342804129</v>
+        <f>STDEV(H4:J4)</f>
+        <v>0.17506152107356859</v>
       </c>
       <c r="F20">
-        <v>0.16806999999999661</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+        <f>E20/SQRT(COUNT(H4:J4))</f>
+        <v>0.10107181631657018</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21">
-        <v>7.862200000000005</v>
+        <f t="shared" ref="C21:C23" si="4">AVERAGE(H5:J5)</f>
+        <v>8.180199111111115</v>
       </c>
       <c r="D21">
-        <v>72811503.67067495</v>
+        <f t="shared" ref="D21:D23" si="5">10^C21</f>
+        <v>151425533.03757924</v>
       </c>
       <c r="E21">
-        <v>1.0367675050480452</v>
+        <f t="shared" ref="E21:E23" si="6">STDEV(H5:J5)</f>
+        <v>0.91695895969456687</v>
       </c>
       <c r="F21">
-        <v>0.73310533333333083</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F21:F23" si="7">E21/SQRT(COUNT(H5:J5))</f>
+        <v>0.52940650221549745</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22">
-        <v>9.0090776666666645</v>
+        <f t="shared" si="4"/>
+        <v>8.9639922222222221</v>
       </c>
       <c r="D22">
-        <v>1021122078.8371067</v>
+        <f t="shared" si="5"/>
+        <v>920433087.57384813</v>
       </c>
       <c r="E22">
-        <v>0.80247615838326269</v>
+        <f t="shared" si="6"/>
+        <v>0.57278450074093157</v>
       </c>
       <c r="F22">
-        <v>0.56743633333333499</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>0.33069728569042228</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23">
-        <v>8.2415579999999942</v>
+        <f t="shared" si="4"/>
+        <v>8.2367559999999944</v>
       </c>
       <c r="D23">
-        <v>174404625.91787061</v>
+        <f t="shared" si="5"/>
+        <v>172486853.55036929</v>
       </c>
       <c r="E23">
-        <v>0.93942907116799568</v>
+        <f t="shared" si="6"/>
+        <v>0.66432873450557706</v>
       </c>
       <c r="F23">
-        <v>0.6642766666666694</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>0.38355037369719835</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>